<commit_message>
add undo method, change fexc constructor
</commit_message>
<xml_diff>
--- a/manual/mfileslist.xlsx
+++ b/manual/mfileslist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="98">
   <si>
     <t xml:space="preserve">fex-metrica/fexSDK/dev/old/annotate/fex_emographs.m             </t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>####</t>
+  </si>
+  <si>
+    <t>nan</t>
   </si>
 </sst>
 </file>
@@ -590,8 +593,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -691,7 +698,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -716,6 +723,8 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -740,6 +749,8 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1072,8 +1083,8 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1119,7 +1130,9 @@
       <c r="D2" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:6">
@@ -1135,7 +1148,9 @@
       <c r="D3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="13"/>
+      <c r="E3" s="13" t="s">
+        <v>97</v>
+      </c>
       <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6">
@@ -1151,7 +1166,9 @@
       <c r="D4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="13"/>
+      <c r="E4" s="13" t="s">
+        <v>97</v>
+      </c>
       <c r="F4" s="17"/>
     </row>
     <row r="5" spans="1:6">
@@ -1167,7 +1184,9 @@
       <c r="D5" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="13"/>
+      <c r="E5" s="13" t="s">
+        <v>97</v>
+      </c>
       <c r="F5" s="17"/>
     </row>
     <row r="6" spans="1:6">
@@ -1183,7 +1202,9 @@
       <c r="D6" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="13"/>
+      <c r="E6" s="13" t="s">
+        <v>97</v>
+      </c>
       <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:6">
@@ -1199,7 +1220,9 @@
       <c r="D7" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="13"/>
+      <c r="E7" s="13" t="s">
+        <v>97</v>
+      </c>
       <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:6">
@@ -1215,7 +1238,9 @@
       <c r="D8" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="13"/>
+      <c r="E8" s="13" t="s">
+        <v>97</v>
+      </c>
       <c r="F8" s="17"/>
     </row>
     <row r="9" spans="1:6">
@@ -1287,7 +1312,9 @@
       <c r="D12" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="13"/>
+      <c r="E12" s="13" t="s">
+        <v>97</v>
+      </c>
       <c r="F12" s="17"/>
     </row>
     <row r="13" spans="1:6">

</xml_diff>